<commit_message>
update MIMAG and MIMS template
</commit_message>
<xml_diff>
--- a/templates/dataplant/MIxS/MIMS_-_Metagenomics.xlsx
+++ b/templates/dataplant/MIxS/MIMS_-_Metagenomics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Template that includes the minimum required information to describe a metagenomics experiment, based on the mimimum information about a metagenome sequence (MIMS) standard. This template should be combined with the MIxS - sample information template to contain all required information.</t>
+    <t>Template that includes the minimum required information to describe a metagenomics experiment, based on the mimimum information about a metagenome sequence (MIMS) standard. This template should be combined with the MIxS - Sample information template to contain all required information.</t>
   </si>
   <si>
     <t>Organisation</t>
@@ -140,7 +140,7 @@
     <t>Input [Sample Name]</t>
   </si>
   <si>
-    <t>Parameter [next generation sequencing instrument model]</t>
+    <t>Component [next generation sequencing instrument model]</t>
   </si>
   <si>
     <t>Term Source REF (DPBO:0000040)</t>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Output [Data]</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>Data Selector Format</t>
   </si>
   <si>
     <t/>
@@ -217,20 +223,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:E2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:E2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:G2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:G2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="7">
     <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Parameter [next generation sequencing instrument model]" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Component [next generation sequencing instrument model]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (DPBO:0000040)" totalsRowFunction="none"/>
     <tableColumn id="4" name="Term Accession Number (DPBO:0000040)" totalsRowFunction="none"/>
     <tableColumn id="5" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Data Format" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Data Selector Format" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -724,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -743,22 +753,34 @@
       <c r="E1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>